<commit_message>
Initial data commit successfully
</commit_message>
<xml_diff>
--- a/backend/Prueba.xlsx
+++ b/backend/Prueba.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlo\Documents\Facultad\Asignaturas\Organización del Trabajo\App\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5D6E9405-CC77-486A-BCE9-8419BC433014}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{979CD57B-0695-4B36-82E5-E2A4D0423377}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="681" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4442" uniqueCount="2013">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4436" uniqueCount="2008">
   <si>
     <t>subject_code</t>
   </si>
@@ -4655,12 +4655,6 @@
   </si>
   <si>
     <t>Behavioural formalisation is the design parameter through which work processes within organisations are standardised.</t>
-  </si>
-  <si>
-    <t>La formalización del comportamiento suele aplicarse a los puestos denominados "no cualificados", es decir, puestos que se encuentran especializados horizontalmente (realizan pocas tareas) y especializados verticalmente (tienen poca capacidad de decisión).</t>
-  </si>
-  <si>
-    <t>Behavioural formalisation is usually applied to so-called "unskilled" positions, i.e. positions that are horizontally specialised (they perform few tasks) and vertically specialised (they have little decision-making power).</t>
   </si>
   <si>
     <t>La formalización del comportamiento da lugar a que las estructuras sean rígidas, es decir, nos encontraríamos ante estructuras burocráticas.</t>
@@ -6063,12 +6057,6 @@
     <t>Organisations that use functional grouping bases often use the action planning system as a liaison device to coordinate units</t>
   </si>
   <si>
-    <t>Cuando las organizaciones usan la base de agrupación funcional, estas suelen descentralizarse vertical y selectivamente</t>
-  </si>
-  <si>
-    <t>When organisations use a functional grouping basis, they tend to decentralise vertically and selectively</t>
-  </si>
-  <si>
     <t>Las organizaciones que utilizan bases de agrupación por mercados, suelen utilizar el sistema de control del rendimiento como dispositivo de enlace para coordinar las unidades</t>
   </si>
   <si>
@@ -6115,9 +6103,6 @@
   </si>
   <si>
     <t>A diversified environment is, by definition, a complex environment, as more knowledge is needed to understand it</t>
-  </si>
-  <si>
-    <t>La extrema hostilidad fuerza a la centralización de la toma de decisiones para poder dar respuestas rápidas, adecuadas y homogéneas</t>
   </si>
   <si>
     <t>Un entorno hostil (alta rivalidad) es, por definición, un entorno dinámico (impredictible)</t>
@@ -6729,25 +6714,25 @@
         <v>100</v>
       </c>
       <c r="B2" t="s">
+        <v>1560</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1561</v>
+      </c>
+      <c r="D2" t="s">
         <v>1562</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>1563</v>
-      </c>
-      <c r="D2" t="s">
-        <v>1564</v>
-      </c>
-      <c r="E2" t="s">
-        <v>1565</v>
       </c>
       <c r="F2">
         <v>10</v>
       </c>
       <c r="G2" t="s">
-        <v>1566</v>
+        <v>1564</v>
       </c>
       <c r="H2" t="s">
-        <v>1567</v>
+        <v>1565</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
@@ -6755,28 +6740,28 @@
         <v>101</v>
       </c>
       <c r="B3" t="s">
+        <v>1566</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1567</v>
+      </c>
+      <c r="D3" t="s">
         <v>1568</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
         <v>1569</v>
-      </c>
-      <c r="D3" t="s">
-        <v>1570</v>
-      </c>
-      <c r="E3" t="s">
-        <v>1571</v>
       </c>
       <c r="F3">
         <v>10</v>
       </c>
       <c r="G3" t="s">
-        <v>1572</v>
+        <v>1570</v>
       </c>
       <c r="H3" t="s">
-        <v>1573</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
+        <v>1571</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>63</v>
       </c>
@@ -6786,20 +6771,20 @@
       <c r="C4" t="s">
         <v>125</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>1574</v>
+      <c r="D4" t="s">
+        <v>1572</v>
       </c>
       <c r="E4" t="s">
-        <v>1575</v>
+        <v>1573</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>1576</v>
+        <v>1574</v>
       </c>
       <c r="H4" t="s">
-        <v>1577</v>
+        <v>1575</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
@@ -6813,19 +6798,19 @@
         <v>22</v>
       </c>
       <c r="D5" t="s">
-        <v>1578</v>
+        <v>1576</v>
       </c>
       <c r="E5" t="s">
-        <v>1579</v>
+        <v>1577</v>
       </c>
       <c r="F5">
         <v>1</v>
       </c>
       <c r="G5" t="s">
-        <v>1580</v>
+        <v>1578</v>
       </c>
       <c r="H5" t="s">
-        <v>1581</v>
+        <v>1579</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
@@ -6839,19 +6824,19 @@
         <v>24</v>
       </c>
       <c r="D6" t="s">
-        <v>1582</v>
+        <v>1580</v>
       </c>
       <c r="E6" t="s">
-        <v>1583</v>
+        <v>1581</v>
       </c>
       <c r="F6">
         <v>1</v>
       </c>
       <c r="G6" t="s">
-        <v>1584</v>
+        <v>1582</v>
       </c>
       <c r="H6" t="s">
-        <v>1585</v>
+        <v>1583</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
@@ -6865,19 +6850,19 @@
         <v>139</v>
       </c>
       <c r="D7" t="s">
-        <v>1586</v>
+        <v>1584</v>
       </c>
       <c r="E7" t="s">
-        <v>1587</v>
+        <v>1585</v>
       </c>
       <c r="F7">
         <v>1</v>
       </c>
       <c r="G7" t="s">
-        <v>1588</v>
+        <v>1586</v>
       </c>
       <c r="H7" t="s">
-        <v>1589</v>
+        <v>1587</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
@@ -6891,19 +6876,19 @@
         <v>26</v>
       </c>
       <c r="D8" t="s">
-        <v>1590</v>
+        <v>1588</v>
       </c>
       <c r="E8" t="s">
-        <v>1591</v>
+        <v>1589</v>
       </c>
       <c r="F8">
         <v>1</v>
       </c>
       <c r="G8" t="s">
-        <v>1592</v>
+        <v>1590</v>
       </c>
       <c r="H8" t="s">
-        <v>1593</v>
+        <v>1591</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
@@ -6917,19 +6902,19 @@
         <v>28</v>
       </c>
       <c r="D9" t="s">
-        <v>1594</v>
+        <v>1592</v>
       </c>
       <c r="E9" t="s">
-        <v>1595</v>
+        <v>1593</v>
       </c>
       <c r="F9">
         <v>1</v>
       </c>
       <c r="G9" t="s">
-        <v>1596</v>
+        <v>1594</v>
       </c>
       <c r="H9" t="s">
-        <v>1597</v>
+        <v>1595</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
@@ -6943,19 +6928,19 @@
         <v>30</v>
       </c>
       <c r="D10" t="s">
-        <v>1598</v>
+        <v>1596</v>
       </c>
       <c r="E10" t="s">
-        <v>1599</v>
+        <v>1597</v>
       </c>
       <c r="F10">
         <v>1</v>
       </c>
       <c r="G10" t="s">
-        <v>1600</v>
+        <v>1598</v>
       </c>
       <c r="H10" t="s">
-        <v>1601</v>
+        <v>1599</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
@@ -6969,22 +6954,22 @@
         <v>32</v>
       </c>
       <c r="D11" t="s">
-        <v>1602</v>
+        <v>1600</v>
       </c>
       <c r="E11" t="s">
-        <v>1603</v>
+        <v>1601</v>
       </c>
       <c r="F11">
         <v>1</v>
       </c>
       <c r="G11" t="s">
-        <v>1604</v>
+        <v>1602</v>
       </c>
       <c r="H11" t="s">
-        <v>1605</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
+        <v>1603</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>64</v>
       </c>
@@ -6994,20 +6979,20 @@
       <c r="C12" t="s">
         <v>127</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>1606</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>1607</v>
+      <c r="D12" t="s">
+        <v>1604</v>
+      </c>
+      <c r="E12" t="s">
+        <v>1605</v>
       </c>
       <c r="F12">
         <v>2</v>
       </c>
-      <c r="G12" s="2" t="s">
-        <v>1608</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>1609</v>
+      <c r="G12" t="s">
+        <v>1606</v>
+      </c>
+      <c r="H12" t="s">
+        <v>1607</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
@@ -7021,19 +7006,19 @@
         <v>34</v>
       </c>
       <c r="D13" t="s">
-        <v>1610</v>
+        <v>1608</v>
       </c>
       <c r="E13" t="s">
-        <v>1611</v>
+        <v>1609</v>
       </c>
       <c r="F13">
         <v>2</v>
       </c>
       <c r="G13" t="s">
-        <v>1612</v>
+        <v>1610</v>
       </c>
       <c r="H13" t="s">
-        <v>1613</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
@@ -7047,19 +7032,19 @@
         <v>36</v>
       </c>
       <c r="D14" t="s">
-        <v>1614</v>
+        <v>1612</v>
       </c>
       <c r="E14" t="s">
-        <v>1615</v>
+        <v>1613</v>
       </c>
       <c r="F14">
         <v>2</v>
       </c>
       <c r="G14" t="s">
-        <v>1616</v>
+        <v>1614</v>
       </c>
       <c r="H14" t="s">
-        <v>1617</v>
+        <v>1615</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
@@ -7073,19 +7058,19 @@
         <v>38</v>
       </c>
       <c r="D15" t="s">
-        <v>1618</v>
+        <v>1616</v>
       </c>
       <c r="E15" t="s">
-        <v>1619</v>
+        <v>1617</v>
       </c>
       <c r="F15">
         <v>2</v>
       </c>
       <c r="G15" t="s">
-        <v>1620</v>
+        <v>1618</v>
       </c>
       <c r="H15" t="s">
-        <v>1621</v>
+        <v>1619</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
@@ -7099,19 +7084,19 @@
         <v>40</v>
       </c>
       <c r="D16" t="s">
-        <v>1622</v>
+        <v>1620</v>
       </c>
       <c r="E16" t="s">
-        <v>1623</v>
+        <v>1621</v>
       </c>
       <c r="F16">
         <v>2</v>
       </c>
       <c r="G16" t="s">
-        <v>1624</v>
+        <v>1622</v>
       </c>
       <c r="H16" t="s">
-        <v>1625</v>
+        <v>1623</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
@@ -7125,19 +7110,19 @@
         <v>42</v>
       </c>
       <c r="D17" t="s">
-        <v>1626</v>
+        <v>1624</v>
       </c>
       <c r="E17" t="s">
-        <v>1627</v>
+        <v>1625</v>
       </c>
       <c r="F17">
         <v>2</v>
       </c>
       <c r="G17" t="s">
-        <v>1628</v>
+        <v>1626</v>
       </c>
       <c r="H17" t="s">
-        <v>1629</v>
+        <v>1627</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
@@ -7151,19 +7136,19 @@
         <v>129</v>
       </c>
       <c r="D18" t="s">
-        <v>1630</v>
+        <v>1628</v>
       </c>
       <c r="E18" t="s">
-        <v>1631</v>
+        <v>1629</v>
       </c>
       <c r="F18">
         <v>11</v>
       </c>
       <c r="G18" t="s">
-        <v>1632</v>
+        <v>1630</v>
       </c>
       <c r="H18" t="s">
-        <v>1633</v>
+        <v>1631</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
@@ -7171,25 +7156,25 @@
         <v>12</v>
       </c>
       <c r="B19" t="s">
+        <v>1632</v>
+      </c>
+      <c r="C19" t="s">
+        <v>1633</v>
+      </c>
+      <c r="D19" t="s">
         <v>1634</v>
       </c>
-      <c r="C19" t="s">
+      <c r="E19" t="s">
         <v>1635</v>
-      </c>
-      <c r="D19" t="s">
-        <v>1636</v>
-      </c>
-      <c r="E19" t="s">
-        <v>1637</v>
       </c>
       <c r="F19">
         <v>3</v>
       </c>
       <c r="G19" t="s">
-        <v>1638</v>
+        <v>1636</v>
       </c>
       <c r="H19" t="s">
-        <v>1639</v>
+        <v>1637</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
@@ -7203,19 +7188,19 @@
         <v>44</v>
       </c>
       <c r="D20" t="s">
-        <v>1640</v>
+        <v>1638</v>
       </c>
       <c r="E20" t="s">
-        <v>1641</v>
+        <v>1639</v>
       </c>
       <c r="F20">
         <v>3</v>
       </c>
       <c r="G20" t="s">
-        <v>1642</v>
+        <v>1640</v>
       </c>
       <c r="H20" t="s">
-        <v>1643</v>
+        <v>1641</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
@@ -7223,25 +7208,25 @@
         <v>15</v>
       </c>
       <c r="B21" t="s">
+        <v>1642</v>
+      </c>
+      <c r="C21" t="s">
+        <v>1643</v>
+      </c>
+      <c r="D21" t="s">
         <v>1644</v>
       </c>
-      <c r="C21" t="s">
+      <c r="E21" t="s">
         <v>1645</v>
-      </c>
-      <c r="D21" t="s">
-        <v>1646</v>
-      </c>
-      <c r="E21" t="s">
-        <v>1647</v>
       </c>
       <c r="F21">
         <v>3</v>
       </c>
       <c r="G21" t="s">
-        <v>1648</v>
+        <v>1646</v>
       </c>
       <c r="H21" t="s">
-        <v>1649</v>
+        <v>1647</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.35">
@@ -7255,19 +7240,19 @@
         <v>46</v>
       </c>
       <c r="D22" t="s">
-        <v>1650</v>
+        <v>1648</v>
       </c>
       <c r="E22" t="s">
-        <v>1651</v>
+        <v>1649</v>
       </c>
       <c r="F22">
         <v>3</v>
       </c>
       <c r="G22" t="s">
-        <v>1652</v>
+        <v>1650</v>
       </c>
       <c r="H22" t="s">
-        <v>1653</v>
+        <v>1651</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.35">
@@ -7281,19 +7266,19 @@
         <v>48</v>
       </c>
       <c r="D23" t="s">
-        <v>1654</v>
+        <v>1652</v>
       </c>
       <c r="E23" t="s">
-        <v>1655</v>
+        <v>1653</v>
       </c>
       <c r="F23">
         <v>3</v>
       </c>
       <c r="G23" t="s">
-        <v>1656</v>
+        <v>1654</v>
       </c>
       <c r="H23" t="s">
-        <v>1657</v>
+        <v>1655</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.35">
@@ -7307,19 +7292,19 @@
         <v>51</v>
       </c>
       <c r="D24" t="s">
-        <v>1658</v>
+        <v>1656</v>
       </c>
       <c r="E24" t="s">
-        <v>1659</v>
+        <v>1657</v>
       </c>
       <c r="F24">
         <v>3</v>
       </c>
       <c r="G24" t="s">
-        <v>1660</v>
+        <v>1658</v>
       </c>
       <c r="H24" t="s">
-        <v>1661</v>
+        <v>1659</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
@@ -7333,19 +7318,19 @@
         <v>168</v>
       </c>
       <c r="D25" t="s">
-        <v>1662</v>
+        <v>1660</v>
       </c>
       <c r="E25" t="s">
-        <v>1663</v>
+        <v>1661</v>
       </c>
       <c r="F25">
         <v>3</v>
       </c>
       <c r="G25" t="s">
-        <v>1664</v>
+        <v>1662</v>
       </c>
       <c r="H25" t="s">
-        <v>1665</v>
+        <v>1663</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.35">
@@ -7359,19 +7344,19 @@
         <v>53</v>
       </c>
       <c r="D26" t="s">
-        <v>1666</v>
+        <v>1664</v>
       </c>
       <c r="E26" t="s">
-        <v>1667</v>
+        <v>1665</v>
       </c>
       <c r="F26">
         <v>3</v>
       </c>
       <c r="G26" t="s">
-        <v>1668</v>
+        <v>1666</v>
       </c>
       <c r="H26" t="s">
-        <v>1669</v>
+        <v>1667</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
@@ -7385,19 +7370,19 @@
         <v>63</v>
       </c>
       <c r="D27" t="s">
-        <v>1670</v>
+        <v>1668</v>
       </c>
       <c r="E27" t="s">
-        <v>1671</v>
+        <v>1669</v>
       </c>
       <c r="F27">
         <v>4</v>
       </c>
       <c r="G27" t="s">
-        <v>1672</v>
+        <v>1670</v>
       </c>
       <c r="H27" t="s">
-        <v>1673</v>
+        <v>1671</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.35">
@@ -7411,19 +7396,19 @@
         <v>65</v>
       </c>
       <c r="D28" t="s">
-        <v>1674</v>
+        <v>1672</v>
       </c>
       <c r="E28" t="s">
-        <v>1675</v>
+        <v>1673</v>
       </c>
       <c r="F28">
         <v>4</v>
       </c>
       <c r="G28" t="s">
-        <v>1676</v>
+        <v>1674</v>
       </c>
       <c r="H28" t="s">
-        <v>1677</v>
+        <v>1675</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.35">
@@ -7437,19 +7422,19 @@
         <v>67</v>
       </c>
       <c r="D29" t="s">
-        <v>1678</v>
+        <v>1676</v>
       </c>
       <c r="E29" t="s">
-        <v>1679</v>
+        <v>1677</v>
       </c>
       <c r="F29">
         <v>4</v>
       </c>
       <c r="G29" t="s">
-        <v>1680</v>
+        <v>1678</v>
       </c>
       <c r="H29" t="s">
-        <v>1681</v>
+        <v>1679</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.35">
@@ -7463,19 +7448,19 @@
         <v>55</v>
       </c>
       <c r="D30" t="s">
-        <v>1682</v>
+        <v>1680</v>
       </c>
       <c r="E30" t="s">
-        <v>1683</v>
+        <v>1681</v>
       </c>
       <c r="F30">
         <v>4</v>
       </c>
       <c r="G30" t="s">
-        <v>1684</v>
+        <v>1682</v>
       </c>
       <c r="H30" t="s">
-        <v>1685</v>
+        <v>1683</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.35">
@@ -7489,19 +7474,19 @@
         <v>57</v>
       </c>
       <c r="D31" t="s">
-        <v>1686</v>
+        <v>1684</v>
       </c>
       <c r="E31" t="s">
-        <v>1687</v>
+        <v>1685</v>
       </c>
       <c r="F31">
         <v>4</v>
       </c>
       <c r="G31" t="s">
-        <v>1688</v>
+        <v>1686</v>
       </c>
       <c r="H31" t="s">
-        <v>1689</v>
+        <v>1687</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.35">
@@ -7515,19 +7500,19 @@
         <v>59</v>
       </c>
       <c r="D32" t="s">
-        <v>1690</v>
+        <v>1688</v>
       </c>
       <c r="E32" t="s">
-        <v>1691</v>
+        <v>1689</v>
       </c>
       <c r="F32">
         <v>4</v>
       </c>
       <c r="G32" t="s">
-        <v>1692</v>
+        <v>1690</v>
       </c>
       <c r="H32" t="s">
-        <v>1693</v>
+        <v>1691</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.35">
@@ -7541,19 +7526,19 @@
         <v>61</v>
       </c>
       <c r="D33" t="s">
-        <v>1694</v>
+        <v>1692</v>
       </c>
       <c r="E33" t="s">
-        <v>1695</v>
+        <v>1693</v>
       </c>
       <c r="F33">
         <v>4</v>
       </c>
       <c r="G33" t="s">
-        <v>1696</v>
+        <v>1694</v>
       </c>
       <c r="H33" t="s">
-        <v>1697</v>
+        <v>1695</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.35">
@@ -7567,19 +7552,19 @@
         <v>69</v>
       </c>
       <c r="D34" t="s">
-        <v>1698</v>
+        <v>1696</v>
       </c>
       <c r="E34" t="s">
-        <v>1699</v>
+        <v>1697</v>
       </c>
       <c r="F34">
         <v>5</v>
       </c>
       <c r="G34" t="s">
-        <v>1700</v>
+        <v>1698</v>
       </c>
       <c r="H34" t="s">
-        <v>1701</v>
+        <v>1699</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.35">
@@ -7593,19 +7578,19 @@
         <v>137</v>
       </c>
       <c r="D35" t="s">
-        <v>1702</v>
+        <v>1700</v>
       </c>
       <c r="E35" t="s">
-        <v>1703</v>
+        <v>1701</v>
       </c>
       <c r="F35">
         <v>5</v>
       </c>
       <c r="G35" t="s">
-        <v>1704</v>
+        <v>1702</v>
       </c>
       <c r="H35" t="s">
-        <v>1705</v>
+        <v>1703</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.35">
@@ -7619,19 +7604,19 @@
         <v>135</v>
       </c>
       <c r="D36" t="s">
-        <v>1706</v>
+        <v>1704</v>
       </c>
       <c r="E36" t="s">
-        <v>1707</v>
+        <v>1705</v>
       </c>
       <c r="F36">
         <v>5</v>
       </c>
       <c r="G36" t="s">
-        <v>1708</v>
+        <v>1706</v>
       </c>
       <c r="H36" t="s">
-        <v>1709</v>
+        <v>1707</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.35">
@@ -7645,19 +7630,19 @@
         <v>71</v>
       </c>
       <c r="D37" t="s">
-        <v>1710</v>
+        <v>1708</v>
       </c>
       <c r="E37" t="s">
-        <v>1711</v>
+        <v>1709</v>
       </c>
       <c r="F37">
         <v>5</v>
       </c>
       <c r="G37" t="s">
-        <v>1712</v>
+        <v>1710</v>
       </c>
       <c r="H37" t="s">
-        <v>1713</v>
+        <v>1711</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.35">
@@ -7671,19 +7656,19 @@
         <v>150</v>
       </c>
       <c r="D38" t="s">
-        <v>1714</v>
+        <v>1712</v>
       </c>
       <c r="E38" t="s">
-        <v>1715</v>
+        <v>1713</v>
       </c>
       <c r="F38">
         <v>5</v>
       </c>
       <c r="G38" t="s">
-        <v>1716</v>
+        <v>1714</v>
       </c>
       <c r="H38" t="s">
-        <v>1717</v>
+        <v>1715</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.35">
@@ -7697,19 +7682,19 @@
         <v>141</v>
       </c>
       <c r="D39" t="s">
-        <v>1718</v>
+        <v>1716</v>
       </c>
       <c r="E39" t="s">
-        <v>1719</v>
+        <v>1717</v>
       </c>
       <c r="F39">
         <v>5</v>
       </c>
       <c r="G39" t="s">
-        <v>1720</v>
+        <v>1718</v>
       </c>
       <c r="H39" t="s">
-        <v>1721</v>
+        <v>1719</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.35">
@@ -7722,20 +7707,20 @@
       <c r="C40" t="s">
         <v>154</v>
       </c>
-      <c r="D40" s="2" t="s">
-        <v>1722</v>
+      <c r="D40" t="s">
+        <v>1720</v>
       </c>
       <c r="E40" t="s">
-        <v>1723</v>
+        <v>1721</v>
       </c>
       <c r="F40">
         <v>5</v>
       </c>
       <c r="G40" t="s">
-        <v>1724</v>
+        <v>1722</v>
       </c>
       <c r="H40" t="s">
-        <v>1725</v>
+        <v>1723</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.35">
@@ -7749,19 +7734,19 @@
         <v>143</v>
       </c>
       <c r="D41" t="s">
-        <v>1726</v>
+        <v>1724</v>
       </c>
       <c r="E41" t="s">
-        <v>1727</v>
+        <v>1725</v>
       </c>
       <c r="F41">
         <v>5</v>
       </c>
       <c r="G41" t="s">
-        <v>1728</v>
+        <v>1726</v>
       </c>
       <c r="H41" t="s">
-        <v>1729</v>
+        <v>1727</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.35">
@@ -7774,20 +7759,20 @@
       <c r="C42" t="s">
         <v>145</v>
       </c>
-      <c r="D42" s="2" t="s">
-        <v>1730</v>
+      <c r="D42" t="s">
+        <v>1728</v>
       </c>
       <c r="E42" t="s">
-        <v>1731</v>
+        <v>1729</v>
       </c>
       <c r="F42">
         <v>5</v>
       </c>
       <c r="G42" t="s">
-        <v>1732</v>
+        <v>1730</v>
       </c>
       <c r="H42" t="s">
-        <v>1733</v>
+        <v>1731</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.35">
@@ -7801,19 +7786,19 @@
         <v>152</v>
       </c>
       <c r="D43" t="s">
-        <v>1734</v>
+        <v>1732</v>
       </c>
       <c r="E43" t="s">
-        <v>1735</v>
+        <v>1733</v>
       </c>
       <c r="F43">
         <v>5</v>
       </c>
       <c r="G43" t="s">
-        <v>1736</v>
+        <v>1734</v>
       </c>
       <c r="H43" t="s">
-        <v>1737</v>
+        <v>1735</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.35">
@@ -7827,19 +7812,19 @@
         <v>117</v>
       </c>
       <c r="D44" t="s">
-        <v>1738</v>
+        <v>1736</v>
       </c>
       <c r="E44" t="s">
-        <v>1739</v>
+        <v>1737</v>
       </c>
       <c r="F44">
         <v>5</v>
       </c>
       <c r="G44" t="s">
-        <v>1740</v>
+        <v>1738</v>
       </c>
       <c r="H44" t="s">
-        <v>1741</v>
+        <v>1739</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.35">
@@ -7853,19 +7838,19 @@
         <v>133</v>
       </c>
       <c r="D45" t="s">
-        <v>1742</v>
+        <v>1740</v>
       </c>
       <c r="E45" t="s">
-        <v>1743</v>
+        <v>1741</v>
       </c>
       <c r="F45">
         <v>6</v>
       </c>
       <c r="G45" t="s">
-        <v>1744</v>
+        <v>1742</v>
       </c>
       <c r="H45" t="s">
-        <v>1745</v>
+        <v>1743</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.35">
@@ -7879,19 +7864,19 @@
         <v>73</v>
       </c>
       <c r="D46" t="s">
-        <v>1746</v>
+        <v>1744</v>
       </c>
       <c r="E46" t="s">
-        <v>1747</v>
+        <v>1745</v>
       </c>
       <c r="F46">
         <v>6</v>
       </c>
       <c r="G46" t="s">
-        <v>1748</v>
+        <v>1746</v>
       </c>
       <c r="H46" t="s">
-        <v>1749</v>
+        <v>1747</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.35">
@@ -7905,19 +7890,19 @@
         <v>131</v>
       </c>
       <c r="D47" t="s">
-        <v>1750</v>
+        <v>1748</v>
       </c>
       <c r="E47" t="s">
-        <v>1751</v>
+        <v>1749</v>
       </c>
       <c r="F47">
         <v>7</v>
       </c>
       <c r="G47" t="s">
-        <v>1752</v>
+        <v>1750</v>
       </c>
       <c r="H47" t="s">
-        <v>1753</v>
+        <v>1751</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.35">
@@ -7931,19 +7916,19 @@
         <v>81</v>
       </c>
       <c r="D48" t="s">
-        <v>1754</v>
+        <v>1752</v>
       </c>
       <c r="E48" t="s">
-        <v>1755</v>
+        <v>1753</v>
       </c>
       <c r="F48">
         <v>7</v>
       </c>
       <c r="G48" t="s">
-        <v>1756</v>
+        <v>1754</v>
       </c>
       <c r="H48" t="s">
-        <v>1757</v>
+        <v>1755</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.35">
@@ -7957,19 +7942,19 @@
         <v>83</v>
       </c>
       <c r="D49" t="s">
-        <v>1758</v>
+        <v>1756</v>
       </c>
       <c r="E49" t="s">
-        <v>1759</v>
+        <v>1757</v>
       </c>
       <c r="F49">
         <v>7</v>
       </c>
       <c r="G49" t="s">
-        <v>1760</v>
+        <v>1758</v>
       </c>
       <c r="H49" t="s">
-        <v>1761</v>
+        <v>1759</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.35">
@@ -7983,19 +7968,19 @@
         <v>85</v>
       </c>
       <c r="D50" t="s">
-        <v>1762</v>
+        <v>1760</v>
       </c>
       <c r="E50" t="s">
-        <v>1763</v>
+        <v>1761</v>
       </c>
       <c r="F50">
         <v>7</v>
       </c>
       <c r="G50" t="s">
-        <v>1764</v>
+        <v>1762</v>
       </c>
       <c r="H50" t="s">
-        <v>1765</v>
+        <v>1763</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.35">
@@ -8009,19 +7994,19 @@
         <v>89</v>
       </c>
       <c r="D51" t="s">
-        <v>1766</v>
+        <v>1764</v>
       </c>
       <c r="E51" t="s">
-        <v>1767</v>
+        <v>1765</v>
       </c>
       <c r="F51">
         <v>7</v>
       </c>
       <c r="G51" t="s">
-        <v>1768</v>
+        <v>1766</v>
       </c>
       <c r="H51" t="s">
-        <v>1769</v>
+        <v>1767</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.35">
@@ -8035,19 +8020,19 @@
         <v>87</v>
       </c>
       <c r="D52" t="s">
-        <v>1770</v>
+        <v>1768</v>
       </c>
       <c r="E52" t="s">
-        <v>1771</v>
+        <v>1769</v>
       </c>
       <c r="F52">
         <v>7</v>
       </c>
       <c r="G52" t="s">
-        <v>1772</v>
+        <v>1770</v>
       </c>
       <c r="H52" t="s">
-        <v>1773</v>
+        <v>1771</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.35">
@@ -8061,19 +8046,19 @@
         <v>93</v>
       </c>
       <c r="D53" t="s">
-        <v>1774</v>
+        <v>1772</v>
       </c>
       <c r="E53" t="s">
-        <v>1775</v>
+        <v>1773</v>
       </c>
       <c r="F53">
         <v>7</v>
       </c>
       <c r="G53" t="s">
-        <v>1776</v>
+        <v>1774</v>
       </c>
       <c r="H53" t="s">
-        <v>1777</v>
+        <v>1775</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.35">
@@ -8087,19 +8072,19 @@
         <v>91</v>
       </c>
       <c r="D54" t="s">
-        <v>1778</v>
+        <v>1776</v>
       </c>
       <c r="E54" t="s">
-        <v>1779</v>
+        <v>1777</v>
       </c>
       <c r="F54">
         <v>7</v>
       </c>
       <c r="G54" t="s">
-        <v>1780</v>
+        <v>1778</v>
       </c>
       <c r="H54" t="s">
-        <v>1781</v>
+        <v>1779</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.35">
@@ -8113,19 +8098,19 @@
         <v>97</v>
       </c>
       <c r="D55" t="s">
-        <v>1782</v>
+        <v>1780</v>
       </c>
       <c r="E55" t="s">
-        <v>1783</v>
+        <v>1781</v>
       </c>
       <c r="F55">
         <v>7</v>
       </c>
       <c r="G55" t="s">
-        <v>1784</v>
+        <v>1782</v>
       </c>
       <c r="H55" t="s">
-        <v>1785</v>
+        <v>1783</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.35">
@@ -8139,19 +8124,19 @@
         <v>95</v>
       </c>
       <c r="D56" t="s">
-        <v>1786</v>
+        <v>1784</v>
       </c>
       <c r="E56" t="s">
-        <v>1787</v>
+        <v>1785</v>
       </c>
       <c r="F56">
         <v>7</v>
       </c>
       <c r="G56" t="s">
-        <v>1788</v>
+        <v>1786</v>
       </c>
       <c r="H56" t="s">
-        <v>1789</v>
+        <v>1787</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.35">
@@ -8165,19 +8150,19 @@
         <v>75</v>
       </c>
       <c r="D57" t="s">
-        <v>1790</v>
+        <v>1788</v>
       </c>
       <c r="E57" t="s">
-        <v>1791</v>
+        <v>1789</v>
       </c>
       <c r="F57">
         <v>7</v>
       </c>
       <c r="G57" t="s">
-        <v>1792</v>
+        <v>1790</v>
       </c>
       <c r="H57" t="s">
-        <v>1793</v>
+        <v>1791</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.35">
@@ -8191,19 +8176,19 @@
         <v>77</v>
       </c>
       <c r="D58" t="s">
-        <v>1794</v>
+        <v>1792</v>
       </c>
       <c r="E58" t="s">
-        <v>1795</v>
+        <v>1793</v>
       </c>
       <c r="F58">
         <v>7</v>
       </c>
       <c r="G58" t="s">
-        <v>1796</v>
+        <v>1794</v>
       </c>
       <c r="H58" t="s">
-        <v>1797</v>
+        <v>1795</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.35">
@@ -8217,19 +8202,19 @@
         <v>99</v>
       </c>
       <c r="D59" t="s">
-        <v>1798</v>
+        <v>1796</v>
       </c>
       <c r="E59" t="s">
-        <v>1799</v>
+        <v>1797</v>
       </c>
       <c r="F59">
         <v>7</v>
       </c>
       <c r="G59" t="s">
-        <v>1800</v>
+        <v>1798</v>
       </c>
       <c r="H59" t="s">
-        <v>1801</v>
+        <v>1799</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.35">
@@ -8243,19 +8228,19 @@
         <v>101</v>
       </c>
       <c r="D60" t="s">
-        <v>1802</v>
+        <v>1800</v>
       </c>
       <c r="E60" t="s">
-        <v>1803</v>
+        <v>1801</v>
       </c>
       <c r="F60">
         <v>7</v>
       </c>
       <c r="G60" t="s">
-        <v>1804</v>
+        <v>1802</v>
       </c>
       <c r="H60" t="s">
-        <v>1805</v>
+        <v>1803</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.35">
@@ -8269,19 +8254,19 @@
         <v>103</v>
       </c>
       <c r="D61" t="s">
-        <v>1806</v>
+        <v>1804</v>
       </c>
       <c r="E61" t="s">
-        <v>1807</v>
+        <v>1805</v>
       </c>
       <c r="F61">
         <v>7</v>
       </c>
       <c r="G61" t="s">
-        <v>1808</v>
+        <v>1806</v>
       </c>
       <c r="H61" t="s">
-        <v>1809</v>
+        <v>1807</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.35">
@@ -8295,19 +8280,19 @@
         <v>79</v>
       </c>
       <c r="D62" t="s">
-        <v>1810</v>
+        <v>1808</v>
       </c>
       <c r="E62" t="s">
-        <v>1811</v>
+        <v>1809</v>
       </c>
       <c r="F62">
         <v>7</v>
       </c>
       <c r="G62" t="s">
-        <v>1812</v>
+        <v>1810</v>
       </c>
       <c r="H62" t="s">
-        <v>1813</v>
+        <v>1811</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.35">
@@ -8318,22 +8303,22 @@
         <v>146</v>
       </c>
       <c r="C63" t="s">
+        <v>1812</v>
+      </c>
+      <c r="D63" t="s">
+        <v>1813</v>
+      </c>
+      <c r="E63" t="s">
         <v>1814</v>
-      </c>
-      <c r="D63" t="s">
-        <v>1815</v>
-      </c>
-      <c r="E63" t="s">
-        <v>1816</v>
       </c>
       <c r="F63">
         <v>14</v>
       </c>
       <c r="G63" t="s">
-        <v>1817</v>
+        <v>1815</v>
       </c>
       <c r="H63" t="s">
-        <v>1818</v>
+        <v>1816</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.35">
@@ -8341,16 +8326,16 @@
         <v>88</v>
       </c>
       <c r="B64" t="s">
-        <v>2008</v>
+        <v>2003</v>
       </c>
       <c r="C64" t="s">
-        <v>2009</v>
+        <v>2004</v>
       </c>
       <c r="D64" t="s">
-        <v>2010</v>
+        <v>2005</v>
       </c>
       <c r="E64" t="s">
-        <v>2011</v>
+        <v>2006</v>
       </c>
       <c r="F64">
         <v>14</v>
@@ -8367,19 +8352,19 @@
         <v>123</v>
       </c>
       <c r="D65" t="s">
-        <v>1819</v>
+        <v>1817</v>
       </c>
       <c r="E65" t="s">
-        <v>1820</v>
+        <v>1818</v>
       </c>
       <c r="F65">
         <v>8</v>
       </c>
       <c r="G65" t="s">
-        <v>1821</v>
+        <v>1819</v>
       </c>
       <c r="H65" t="s">
-        <v>1822</v>
+        <v>1820</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.35">
@@ -8393,19 +8378,19 @@
         <v>121</v>
       </c>
       <c r="D66" t="s">
-        <v>1823</v>
+        <v>1821</v>
       </c>
       <c r="E66" t="s">
-        <v>1824</v>
+        <v>1822</v>
       </c>
       <c r="F66">
         <v>8</v>
       </c>
       <c r="G66" t="s">
-        <v>1825</v>
+        <v>1823</v>
       </c>
       <c r="H66" t="s">
-        <v>1826</v>
+        <v>1824</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.35">
@@ -8419,19 +8404,19 @@
         <v>105</v>
       </c>
       <c r="D67" t="s">
-        <v>1827</v>
+        <v>1825</v>
       </c>
       <c r="E67" t="s">
-        <v>1828</v>
+        <v>1826</v>
       </c>
       <c r="F67">
         <v>8</v>
       </c>
       <c r="G67" t="s">
-        <v>1829</v>
+        <v>1827</v>
       </c>
       <c r="H67" t="s">
-        <v>1830</v>
+        <v>1828</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.35">
@@ -8445,19 +8430,19 @@
         <v>107</v>
       </c>
       <c r="D68" t="s">
-        <v>1831</v>
+        <v>1829</v>
       </c>
       <c r="E68" t="s">
-        <v>1832</v>
+        <v>1830</v>
       </c>
       <c r="F68">
         <v>8</v>
       </c>
       <c r="G68" t="s">
-        <v>1833</v>
+        <v>1831</v>
       </c>
       <c r="H68" t="s">
-        <v>1834</v>
+        <v>1832</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.35">
@@ -8471,19 +8456,19 @@
         <v>109</v>
       </c>
       <c r="D69" t="s">
-        <v>1835</v>
+        <v>1833</v>
       </c>
       <c r="E69" t="s">
-        <v>1836</v>
+        <v>1834</v>
       </c>
       <c r="F69">
         <v>8</v>
       </c>
       <c r="G69" t="s">
-        <v>1837</v>
+        <v>1835</v>
       </c>
       <c r="H69" t="s">
-        <v>1838</v>
+        <v>1836</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.35">
@@ -8497,19 +8482,19 @@
         <v>111</v>
       </c>
       <c r="D70" t="s">
-        <v>1839</v>
+        <v>1837</v>
       </c>
       <c r="E70" t="s">
-        <v>1840</v>
+        <v>1838</v>
       </c>
       <c r="F70">
         <v>8</v>
       </c>
       <c r="G70" t="s">
-        <v>1841</v>
+        <v>1839</v>
       </c>
       <c r="H70" t="s">
-        <v>1842</v>
+        <v>1840</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.35">
@@ -8523,19 +8508,19 @@
         <v>113</v>
       </c>
       <c r="D71" t="s">
-        <v>1843</v>
+        <v>1841</v>
       </c>
       <c r="E71" t="s">
-        <v>1844</v>
+        <v>1842</v>
       </c>
       <c r="F71">
         <v>8</v>
       </c>
       <c r="G71" t="s">
-        <v>1845</v>
+        <v>1843</v>
       </c>
       <c r="H71" t="s">
-        <v>1846</v>
+        <v>1844</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.35">
@@ -8549,19 +8534,19 @@
         <v>115</v>
       </c>
       <c r="D72" t="s">
-        <v>1847</v>
+        <v>1845</v>
       </c>
       <c r="E72" t="s">
-        <v>1848</v>
+        <v>1846</v>
       </c>
       <c r="F72">
         <v>8</v>
       </c>
       <c r="G72" t="s">
-        <v>1849</v>
+        <v>1847</v>
       </c>
       <c r="H72" t="s">
-        <v>1850</v>
+        <v>1848</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.35">
@@ -8569,25 +8554,25 @@
         <v>102</v>
       </c>
       <c r="B73" t="s">
+        <v>1849</v>
+      </c>
+      <c r="C73" t="s">
+        <v>1850</v>
+      </c>
+      <c r="D73" t="s">
         <v>1851</v>
       </c>
-      <c r="C73" t="s">
+      <c r="E73" t="s">
         <v>1852</v>
-      </c>
-      <c r="D73" t="s">
-        <v>1853</v>
-      </c>
-      <c r="E73" t="s">
-        <v>1854</v>
       </c>
       <c r="F73">
         <v>9</v>
       </c>
       <c r="G73" t="s">
-        <v>1855</v>
+        <v>1853</v>
       </c>
       <c r="H73" t="s">
-        <v>1856</v>
+        <v>1854</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.35">
@@ -8595,25 +8580,25 @@
         <v>103</v>
       </c>
       <c r="B74" t="s">
+        <v>1855</v>
+      </c>
+      <c r="C74" t="s">
+        <v>1856</v>
+      </c>
+      <c r="D74" t="s">
         <v>1857</v>
       </c>
-      <c r="C74" t="s">
+      <c r="E74" t="s">
         <v>1858</v>
-      </c>
-      <c r="D74" t="s">
-        <v>1859</v>
-      </c>
-      <c r="E74" t="s">
-        <v>1860</v>
       </c>
       <c r="F74">
         <v>9</v>
       </c>
       <c r="G74" t="s">
-        <v>1861</v>
+        <v>1859</v>
       </c>
       <c r="H74" t="s">
-        <v>1862</v>
+        <v>1860</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.35">
@@ -8621,25 +8606,25 @@
         <v>104</v>
       </c>
       <c r="B75" t="s">
+        <v>1861</v>
+      </c>
+      <c r="C75" t="s">
+        <v>1862</v>
+      </c>
+      <c r="D75" t="s">
         <v>1863</v>
       </c>
-      <c r="C75" t="s">
+      <c r="E75" t="s">
         <v>1864</v>
-      </c>
-      <c r="D75" t="s">
-        <v>1865</v>
-      </c>
-      <c r="E75" t="s">
-        <v>1866</v>
       </c>
       <c r="F75">
         <v>9</v>
       </c>
       <c r="G75" t="s">
-        <v>1867</v>
+        <v>1865</v>
       </c>
       <c r="H75" t="s">
-        <v>1868</v>
+        <v>1866</v>
       </c>
     </row>
   </sheetData>
@@ -8700,10 +8685,10 @@
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>1869</v>
+        <v>1867</v>
       </c>
       <c r="G2" t="s">
-        <v>1870</v>
+        <v>1868</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
@@ -8723,10 +8708,10 @@
         <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>1871</v>
+        <v>1869</v>
       </c>
       <c r="G3" t="s">
-        <v>1872</v>
+        <v>1870</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
@@ -8746,10 +8731,10 @@
         <v>3</v>
       </c>
       <c r="F4" t="s">
-        <v>1873</v>
+        <v>1871</v>
       </c>
       <c r="G4" t="s">
-        <v>1874</v>
+        <v>1872</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
@@ -8769,10 +8754,10 @@
         <v>4</v>
       </c>
       <c r="F5" t="s">
-        <v>1875</v>
+        <v>1873</v>
       </c>
       <c r="G5" t="s">
-        <v>1876</v>
+        <v>1874</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
@@ -8792,10 +8777,10 @@
         <v>5</v>
       </c>
       <c r="F6" t="s">
-        <v>1877</v>
+        <v>1875</v>
       </c>
       <c r="G6" t="s">
-        <v>1878</v>
+        <v>1876</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
@@ -8815,10 +8800,10 @@
         <v>6</v>
       </c>
       <c r="F7" t="s">
-        <v>1879</v>
+        <v>1877</v>
       </c>
       <c r="G7" t="s">
-        <v>1880</v>
+        <v>1878</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
@@ -8838,10 +8823,10 @@
         <v>7</v>
       </c>
       <c r="F8" t="s">
-        <v>1881</v>
+        <v>1879</v>
       </c>
       <c r="G8" t="s">
-        <v>1882</v>
+        <v>1880</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
@@ -8861,10 +8846,10 @@
         <v>8</v>
       </c>
       <c r="F9" t="s">
-        <v>1883</v>
+        <v>1881</v>
       </c>
       <c r="G9" t="s">
-        <v>1884</v>
+        <v>1882</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
@@ -8884,10 +8869,10 @@
         <v>9</v>
       </c>
       <c r="F10" t="s">
-        <v>1885</v>
+        <v>1883</v>
       </c>
       <c r="G10" t="s">
-        <v>1886</v>
+        <v>1884</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
@@ -8907,10 +8892,10 @@
         <v>10</v>
       </c>
       <c r="F11" t="s">
-        <v>1887</v>
+        <v>1885</v>
       </c>
       <c r="G11" t="s">
-        <v>1888</v>
+        <v>1886</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
@@ -8930,10 +8915,10 @@
         <v>11</v>
       </c>
       <c r="F12" t="s">
-        <v>1889</v>
+        <v>1887</v>
       </c>
       <c r="G12" t="s">
-        <v>1890</v>
+        <v>1888</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
@@ -8953,10 +8938,10 @@
         <v>12</v>
       </c>
       <c r="F13" t="s">
-        <v>1891</v>
+        <v>1889</v>
       </c>
       <c r="G13" t="s">
-        <v>1892</v>
+        <v>1890</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
@@ -8976,10 +8961,10 @@
         <v>13</v>
       </c>
       <c r="F14" t="s">
-        <v>1893</v>
+        <v>1891</v>
       </c>
       <c r="G14" t="s">
-        <v>1894</v>
+        <v>1892</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
@@ -8999,10 +8984,10 @@
         <v>14</v>
       </c>
       <c r="F15" t="s">
-        <v>1895</v>
+        <v>1893</v>
       </c>
       <c r="G15" t="s">
-        <v>1896</v>
+        <v>1894</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
@@ -9022,10 +9007,10 @@
         <v>15</v>
       </c>
       <c r="F16" t="s">
-        <v>1897</v>
+        <v>1895</v>
       </c>
       <c r="G16" t="s">
-        <v>1898</v>
+        <v>1896</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
@@ -9045,10 +9030,10 @@
         <v>16</v>
       </c>
       <c r="F17" t="s">
-        <v>1899</v>
+        <v>1897</v>
       </c>
       <c r="G17" t="s">
-        <v>1900</v>
+        <v>1898</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
@@ -9068,10 +9053,10 @@
         <v>17</v>
       </c>
       <c r="F18" t="s">
-        <v>1901</v>
+        <v>1899</v>
       </c>
       <c r="G18" t="s">
-        <v>1902</v>
+        <v>1900</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
@@ -9091,10 +9076,10 @@
         <v>18</v>
       </c>
       <c r="F19" t="s">
-        <v>1903</v>
+        <v>1901</v>
       </c>
       <c r="G19" t="s">
-        <v>1904</v>
+        <v>1902</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
@@ -9105,19 +9090,19 @@
         <v>7</v>
       </c>
       <c r="C20" t="s">
-        <v>1905</v>
+        <v>1903</v>
       </c>
       <c r="D20" t="s">
-        <v>1906</v>
+        <v>1904</v>
       </c>
       <c r="E20">
         <v>19</v>
       </c>
       <c r="F20" t="s">
-        <v>1907</v>
+        <v>1905</v>
       </c>
       <c r="G20" t="s">
-        <v>1908</v>
+        <v>1906</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
@@ -9137,10 +9122,10 @@
         <v>20</v>
       </c>
       <c r="F21" t="s">
-        <v>1909</v>
+        <v>1907</v>
       </c>
       <c r="G21" t="s">
-        <v>1910</v>
+        <v>1908</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
@@ -9151,19 +9136,19 @@
         <v>7</v>
       </c>
       <c r="C22" t="s">
-        <v>1911</v>
+        <v>1909</v>
       </c>
       <c r="D22" t="s">
-        <v>1912</v>
+        <v>1910</v>
       </c>
       <c r="E22">
         <v>21</v>
       </c>
       <c r="F22" t="s">
-        <v>1913</v>
+        <v>1911</v>
       </c>
       <c r="G22" t="s">
-        <v>1914</v>
+        <v>1912</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
@@ -9177,16 +9162,16 @@
         <v>174</v>
       </c>
       <c r="D23" t="s">
-        <v>1915</v>
+        <v>1913</v>
       </c>
       <c r="E23">
         <v>22</v>
       </c>
       <c r="F23" t="s">
-        <v>1916</v>
+        <v>1914</v>
       </c>
       <c r="G23" t="s">
-        <v>1917</v>
+        <v>1915</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
@@ -9206,10 +9191,10 @@
         <v>23</v>
       </c>
       <c r="F24" t="s">
-        <v>1918</v>
+        <v>1916</v>
       </c>
       <c r="G24" t="s">
-        <v>1919</v>
+        <v>1917</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
@@ -9229,10 +9214,10 @@
         <v>24</v>
       </c>
       <c r="F25" t="s">
-        <v>1920</v>
+        <v>1918</v>
       </c>
       <c r="G25" t="s">
-        <v>1921</v>
+        <v>1919</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.35">
@@ -9252,10 +9237,10 @@
         <v>25</v>
       </c>
       <c r="F26" t="s">
-        <v>1922</v>
+        <v>1920</v>
       </c>
       <c r="G26" t="s">
-        <v>1923</v>
+        <v>1921</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
@@ -9275,10 +9260,10 @@
         <v>26</v>
       </c>
       <c r="F27" t="s">
-        <v>1924</v>
+        <v>1922</v>
       </c>
       <c r="G27" t="s">
-        <v>1925</v>
+        <v>1923</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
@@ -9298,10 +9283,10 @@
         <v>27</v>
       </c>
       <c r="F28" t="s">
-        <v>1926</v>
+        <v>1924</v>
       </c>
       <c r="G28" t="s">
-        <v>1927</v>
+        <v>1925</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
@@ -9321,10 +9306,10 @@
         <v>28</v>
       </c>
       <c r="F29" t="s">
-        <v>1928</v>
+        <v>1926</v>
       </c>
       <c r="G29" t="s">
-        <v>1929</v>
+        <v>1927</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.35">
@@ -9338,16 +9323,16 @@
         <v>114</v>
       </c>
       <c r="D30" t="s">
-        <v>1930</v>
+        <v>1928</v>
       </c>
       <c r="E30">
         <v>29</v>
       </c>
       <c r="F30" t="s">
-        <v>1931</v>
+        <v>1929</v>
       </c>
       <c r="G30" t="s">
-        <v>1932</v>
+        <v>1930</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.35">
@@ -9367,10 +9352,10 @@
         <v>30</v>
       </c>
       <c r="F31" t="s">
-        <v>1933</v>
+        <v>1931</v>
       </c>
       <c r="G31" t="s">
-        <v>1934</v>
+        <v>1932</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.35">
@@ -9381,19 +9366,19 @@
         <v>9</v>
       </c>
       <c r="C32" t="s">
-        <v>1851</v>
+        <v>1849</v>
       </c>
       <c r="D32" t="s">
-        <v>1852</v>
+        <v>1850</v>
       </c>
       <c r="E32">
         <v>31</v>
       </c>
       <c r="F32" t="s">
-        <v>1935</v>
+        <v>1933</v>
       </c>
       <c r="G32" t="s">
-        <v>1936</v>
+        <v>1934</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.35">
@@ -9404,19 +9389,19 @@
         <v>9</v>
       </c>
       <c r="C33" t="s">
-        <v>1857</v>
+        <v>1855</v>
       </c>
       <c r="D33" t="s">
-        <v>1858</v>
+        <v>1856</v>
       </c>
       <c r="E33">
         <v>32</v>
       </c>
       <c r="F33" t="s">
-        <v>1937</v>
+        <v>1935</v>
       </c>
       <c r="G33" t="s">
-        <v>1938</v>
+        <v>1936</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.35">
@@ -9427,19 +9412,19 @@
         <v>9</v>
       </c>
       <c r="C34" t="s">
-        <v>1863</v>
+        <v>1861</v>
       </c>
       <c r="D34" t="s">
-        <v>1939</v>
+        <v>1937</v>
       </c>
       <c r="E34">
         <v>33</v>
       </c>
       <c r="F34" t="s">
-        <v>1940</v>
+        <v>1938</v>
       </c>
       <c r="G34" t="s">
-        <v>1941</v>
+        <v>1939</v>
       </c>
     </row>
   </sheetData>
@@ -9499,7 +9484,7 @@
         <v>181</v>
       </c>
       <c r="C2" t="s">
-        <v>2012</v>
+        <v>2007</v>
       </c>
       <c r="D2" t="s">
         <v>182</v>
@@ -16459,7 +16444,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="270" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:8" ht="248" x14ac:dyDescent="0.35">
       <c r="A270">
         <v>570</v>
       </c>
@@ -27734,7 +27719,7 @@
         <v>1529</v>
       </c>
       <c r="F2" t="s">
-        <v>1942</v>
+        <v>1940</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -27754,10 +27739,10 @@
         <v>125</v>
       </c>
       <c r="E3" t="s">
-        <v>1943</v>
+        <v>1941</v>
       </c>
       <c r="F3" t="s">
-        <v>1944</v>
+        <v>1942</v>
       </c>
       <c r="G3">
         <v>2</v>
@@ -27780,7 +27765,7 @@
         <v>1530</v>
       </c>
       <c r="F4" t="s">
-        <v>1945</v>
+        <v>1943</v>
       </c>
       <c r="G4">
         <v>3</v>
@@ -27800,10 +27785,10 @@
         <v>129</v>
       </c>
       <c r="E5" t="s">
-        <v>1946</v>
+        <v>1944</v>
       </c>
       <c r="F5" t="s">
-        <v>1947</v>
+        <v>1945</v>
       </c>
       <c r="G5">
         <v>4</v>
@@ -27823,10 +27808,10 @@
         <v>163</v>
       </c>
       <c r="E6" t="s">
-        <v>1948</v>
+        <v>1946</v>
       </c>
       <c r="F6" t="s">
-        <v>1949</v>
+        <v>1947</v>
       </c>
       <c r="G6">
         <v>5</v>
@@ -27846,10 +27831,10 @@
         <v>1532</v>
       </c>
       <c r="E7" t="s">
-        <v>1950</v>
+        <v>1948</v>
       </c>
       <c r="F7" t="s">
-        <v>1951</v>
+        <v>1949</v>
       </c>
       <c r="G7">
         <v>6</v>
@@ -27869,10 +27854,10 @@
         <v>1534</v>
       </c>
       <c r="E8" t="s">
-        <v>1952</v>
+        <v>1950</v>
       </c>
       <c r="F8" t="s">
-        <v>1953</v>
+        <v>1951</v>
       </c>
       <c r="G8">
         <v>7</v>
@@ -27892,10 +27877,10 @@
         <v>173</v>
       </c>
       <c r="E9" t="s">
-        <v>1954</v>
+        <v>1952</v>
       </c>
       <c r="F9" t="s">
-        <v>1955</v>
+        <v>1953</v>
       </c>
       <c r="G9">
         <v>8</v>
@@ -27915,10 +27900,10 @@
         <v>131</v>
       </c>
       <c r="E10" t="s">
-        <v>1956</v>
+        <v>1954</v>
       </c>
       <c r="F10" t="s">
-        <v>1957</v>
+        <v>1955</v>
       </c>
       <c r="G10">
         <v>9</v>
@@ -27938,10 +27923,10 @@
         <v>1536</v>
       </c>
       <c r="E11" t="s">
-        <v>1958</v>
+        <v>1956</v>
       </c>
       <c r="F11" t="s">
-        <v>1959</v>
+        <v>1957</v>
       </c>
       <c r="G11">
         <v>10</v>
@@ -27961,10 +27946,10 @@
         <v>148</v>
       </c>
       <c r="E12" t="s">
-        <v>1960</v>
+        <v>1958</v>
       </c>
       <c r="F12" t="s">
-        <v>1961</v>
+        <v>1959</v>
       </c>
       <c r="G12">
         <v>11</v>
@@ -27984,10 +27969,10 @@
         <v>119</v>
       </c>
       <c r="E13" t="s">
-        <v>1962</v>
+        <v>1960</v>
       </c>
       <c r="F13" t="s">
-        <v>1963</v>
+        <v>1961</v>
       </c>
       <c r="G13">
         <v>12</v>
@@ -28001,7 +27986,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:D36"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -28032,10 +28017,10 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>1964</v>
+        <v>1962</v>
       </c>
       <c r="D2" t="s">
-        <v>1545</v>
+        <v>1543</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -28046,10 +28031,10 @@
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>1965</v>
+        <v>1963</v>
       </c>
       <c r="D3" t="s">
-        <v>1966</v>
+        <v>1964</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -28060,10 +28045,10 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>1967</v>
+        <v>1965</v>
       </c>
       <c r="D4" t="s">
-        <v>1968</v>
+        <v>1966</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
@@ -28074,10 +28059,10 @@
         <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>1546</v>
+        <v>1544</v>
       </c>
       <c r="D5" t="s">
-        <v>1547</v>
+        <v>1545</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
@@ -28088,10 +28073,10 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>1548</v>
+        <v>1546</v>
       </c>
       <c r="D6" t="s">
-        <v>1558</v>
+        <v>1556</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
@@ -28102,10 +28087,10 @@
         <v>80</v>
       </c>
       <c r="C7" t="s">
-        <v>1560</v>
+        <v>1558</v>
       </c>
       <c r="D7" t="s">
-        <v>1561</v>
+        <v>1559</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
@@ -28116,10 +28101,10 @@
         <v>80</v>
       </c>
       <c r="C8" t="s">
-        <v>1555</v>
+        <v>1553</v>
       </c>
       <c r="D8" t="s">
-        <v>1556</v>
+        <v>1554</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
@@ -28130,10 +28115,10 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>1969</v>
+        <v>1967</v>
       </c>
       <c r="D9" t="s">
-        <v>1970</v>
+        <v>1968</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
@@ -28144,10 +28129,10 @@
         <v>4</v>
       </c>
       <c r="C10" t="s">
-        <v>1971</v>
+        <v>1969</v>
       </c>
       <c r="D10" t="s">
-        <v>1972</v>
+        <v>1970</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
@@ -28158,10 +28143,10 @@
         <v>18</v>
       </c>
       <c r="C11" t="s">
-        <v>1553</v>
+        <v>1551</v>
       </c>
       <c r="D11" t="s">
-        <v>1554</v>
+        <v>1552</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
@@ -28186,10 +28171,10 @@
         <v>17</v>
       </c>
       <c r="C13" t="s">
-        <v>1552</v>
+        <v>1550</v>
       </c>
       <c r="D13" t="s">
-        <v>1973</v>
+        <v>1971</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
@@ -28200,32 +28185,32 @@
         <v>62</v>
       </c>
       <c r="C14" t="s">
-        <v>1543</v>
+        <v>1541</v>
       </c>
       <c r="D14" t="s">
-        <v>1544</v>
+        <v>1542</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B15">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="C15" t="s">
-        <v>1541</v>
+        <v>1972</v>
       </c>
       <c r="D15" t="s">
-        <v>1542</v>
+        <v>1973</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B16">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C16" t="s">
         <v>1974</v>
@@ -28236,10 +28221,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B17">
-        <v>79</v>
+        <v>1</v>
       </c>
       <c r="C17" t="s">
         <v>1976</v>
@@ -28250,10 +28235,10 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="B18">
-        <v>77</v>
+        <v>18</v>
       </c>
       <c r="C18" t="s">
         <v>1978</v>
@@ -28264,10 +28249,10 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="B19">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="C19" t="s">
         <v>1980</v>
@@ -28278,10 +28263,10 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B20">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C20" t="s">
         <v>1982</v>
@@ -28292,10 +28277,10 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B21">
-        <v>18</v>
+        <v>61</v>
       </c>
       <c r="C21" t="s">
         <v>1984</v>
@@ -28306,52 +28291,52 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B22">
-        <v>20</v>
+        <v>74</v>
       </c>
       <c r="C22" t="s">
-        <v>1986</v>
+        <v>1547</v>
       </c>
       <c r="D22" t="s">
-        <v>1987</v>
+        <v>1548</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B23">
-        <v>61</v>
+        <v>26</v>
       </c>
       <c r="C23" t="s">
-        <v>1988</v>
+        <v>1986</v>
       </c>
       <c r="D23" t="s">
-        <v>1989</v>
+        <v>1987</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24">
+        <v>43</v>
+      </c>
+      <c r="B24">
         <v>41</v>
       </c>
-      <c r="B24">
-        <v>74</v>
-      </c>
       <c r="C24" t="s">
-        <v>1549</v>
+        <v>1988</v>
       </c>
       <c r="D24" t="s">
-        <v>1550</v>
+        <v>1989</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B25">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="C25" t="s">
         <v>1990</v>
@@ -28362,10 +28347,10 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B26">
-        <v>41</v>
+        <v>18</v>
       </c>
       <c r="C26" t="s">
         <v>1992</v>
@@ -28376,24 +28361,24 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B27">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C27" t="s">
         <v>1994</v>
       </c>
       <c r="D27" t="s">
-        <v>276</v>
+        <v>1549</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28">
-        <v>45</v>
+        <v>74</v>
       </c>
       <c r="B28">
-        <v>40</v>
+        <v>14</v>
       </c>
       <c r="C28" t="s">
         <v>1995</v>
@@ -28404,10 +28389,10 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29">
-        <v>48</v>
+        <v>77</v>
       </c>
       <c r="B29">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="C29" t="s">
         <v>1997</v>
@@ -28418,27 +28403,27 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30">
-        <v>49</v>
+        <v>78</v>
       </c>
       <c r="B30">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="C30" t="s">
         <v>1999</v>
       </c>
       <c r="D30" t="s">
-        <v>1551</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="B31">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C31" t="s">
-        <v>2000</v>
+        <v>1999</v>
       </c>
       <c r="D31" t="s">
         <v>2001</v>
@@ -28446,72 +28431,30 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B32">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C32" t="s">
-        <v>2002</v>
+        <v>1557</v>
       </c>
       <c r="D32" t="s">
-        <v>2003</v>
+        <v>1555</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B33">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C33" t="s">
-        <v>2004</v>
+        <v>1558</v>
       </c>
       <c r="D33" t="s">
-        <v>2005</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A34">
-        <v>78</v>
-      </c>
-      <c r="B34">
-        <v>5</v>
-      </c>
-      <c r="C34" t="s">
-        <v>2004</v>
-      </c>
-      <c r="D34" t="s">
-        <v>2006</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A35">
-        <v>80</v>
-      </c>
-      <c r="B35">
-        <v>2</v>
-      </c>
-      <c r="C35" t="s">
-        <v>1559</v>
-      </c>
-      <c r="D35" t="s">
-        <v>1557</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A36">
-        <v>80</v>
-      </c>
-      <c r="B36">
-        <v>9</v>
-      </c>
-      <c r="C36" t="s">
-        <v>1560</v>
-      </c>
-      <c r="D36" t="s">
-        <v>2007</v>
+        <v>2002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>